<commit_message>
Atualização dos arquivos após alguns ajustes na Main
</commit_message>
<xml_diff>
--- a/Bases/Lista de ações Análise 2025-01-18.xlsx
+++ b/Bases/Lista de ações Análise 2025-01-18.xlsx
@@ -2649,13 +2649,13 @@
         <v>11.32510821884554</v>
       </c>
       <c r="I2">
-        <v>-0.01725281227569931</v>
+        <v>-0.01725280288442166</v>
       </c>
       <c r="J2">
-        <v>12.14238357543945</v>
+        <v>12.14238262176514</v>
       </c>
       <c r="K2">
-        <v>12.07427755172985</v>
+        <v>12.07427660340465</v>
       </c>
       <c r="L2" t="s">
         <v>487</v>
@@ -4283,13 +4283,13 @@
         <v>27.67214569822436</v>
       </c>
       <c r="I45">
-        <v>-0.02883993835758546</v>
+        <v>-0.02883997195536904</v>
       </c>
       <c r="J45">
-        <v>30.34274101257324</v>
+        <v>30.34274291992188</v>
       </c>
       <c r="K45">
-        <v>30.24763268324209</v>
+        <v>30.2476345846122</v>
       </c>
       <c r="L45" t="s">
         <v>530</v>
@@ -5879,7 +5879,7 @@
         <v>20.73937388263526</v>
       </c>
       <c r="I87">
-        <v>-0.08645657212632087</v>
+        <v>-0.08645658821073868</v>
       </c>
       <c r="J87">
         <v>22.49882888793945</v>
@@ -9173,25 +9173,25 @@
         <v>1519310208</v>
       </c>
       <c r="E174">
-        <v>-0.008136398776507816</v>
+        <v>-0.01063313132635392</v>
       </c>
       <c r="F174">
-        <v>5.489487648010254</v>
+        <v>5.588408470153809</v>
       </c>
       <c r="G174">
         <v>5.383333365122478</v>
       </c>
       <c r="H174">
-        <v>5.542122354331217</v>
+        <v>5.641991656325061</v>
       </c>
       <c r="I174">
-        <v>-0.02166095425894028</v>
+        <v>-0.02787984413430601</v>
       </c>
       <c r="J174">
-        <v>6.288296699523926</v>
+        <v>6.401612281799316</v>
       </c>
       <c r="K174">
-        <v>6.248046611248216</v>
+        <v>6.3606368838877</v>
       </c>
       <c r="L174" t="s">
         <v>659</v>

</xml_diff>

<commit_message>
Atualização dos arquivos Python com o código adaptado do Jupyter Notebook
</commit_message>
<xml_diff>
--- a/Bases/Lista de ações Análise 2025-01-18.xlsx
+++ b/Bases/Lista de ações Análise 2025-01-18.xlsx
@@ -2649,13 +2649,13 @@
         <v>11.32510821884554</v>
       </c>
       <c r="I2">
-        <v>-0.01725280288442166</v>
+        <v>-0.01725281227569931</v>
       </c>
       <c r="J2">
-        <v>12.14238262176514</v>
+        <v>12.14238357543945</v>
       </c>
       <c r="K2">
-        <v>12.07427660340465</v>
+        <v>12.07427755172985</v>
       </c>
       <c r="L2" t="s">
         <v>487</v>
@@ -4283,13 +4283,13 @@
         <v>27.67214569822436</v>
       </c>
       <c r="I45">
-        <v>-0.02883997195536904</v>
+        <v>-0.02883993835758546</v>
       </c>
       <c r="J45">
-        <v>30.34274291992188</v>
+        <v>30.34274101257324</v>
       </c>
       <c r="K45">
-        <v>30.2476345846122</v>
+        <v>30.24763268324209</v>
       </c>
       <c r="L45" t="s">
         <v>530</v>
@@ -5879,7 +5879,7 @@
         <v>20.73937388263526</v>
       </c>
       <c r="I87">
-        <v>-0.08645658821073868</v>
+        <v>-0.08645657212632087</v>
       </c>
       <c r="J87">
         <v>22.49882888793945</v>
@@ -6095,25 +6095,25 @@
         <v>43439996928</v>
       </c>
       <c r="E93">
-        <v>0.01300045702419255</v>
+        <v>0.01284729808914427</v>
       </c>
       <c r="F93">
-        <v>14.14503574371338</v>
+        <v>14.14675045013428</v>
       </c>
       <c r="G93">
         <v>14.42333316802979</v>
       </c>
       <c r="H93">
-        <v>14.30807180557233</v>
+        <v>14.30980627574549</v>
       </c>
       <c r="I93">
-        <v>-0.06953861001799555</v>
+        <v>-0.0696466026787482</v>
       </c>
       <c r="J93">
-        <v>15.64170932769775</v>
+        <v>15.64360523223877</v>
       </c>
       <c r="K93">
-        <v>15.66453463126743</v>
+        <v>15.66643330242402</v>
       </c>
       <c r="L93" t="s">
         <v>578</v>

</xml_diff>

<commit_message>
Atualização do Readme com o To-Do
</commit_message>
<xml_diff>
--- a/Bases/Lista de ações Análise 2025-01-18.xlsx
+++ b/Bases/Lista de ações Análise 2025-01-18.xlsx
@@ -6095,25 +6095,25 @@
         <v>43439996928</v>
       </c>
       <c r="E93">
-        <v>0.01284729808914427</v>
+        <v>0.01300045702419255</v>
       </c>
       <c r="F93">
-        <v>14.14675045013428</v>
+        <v>14.14503574371338</v>
       </c>
       <c r="G93">
         <v>14.42333316802979</v>
       </c>
       <c r="H93">
-        <v>14.30980627574549</v>
+        <v>14.30807180557233</v>
       </c>
       <c r="I93">
-        <v>-0.0696466026787482</v>
+        <v>-0.06953861001799555</v>
       </c>
       <c r="J93">
-        <v>15.64360523223877</v>
+        <v>15.64170932769775</v>
       </c>
       <c r="K93">
-        <v>15.66643330242402</v>
+        <v>15.66453463126743</v>
       </c>
       <c r="L93" t="s">
         <v>578</v>

</xml_diff>